<commit_message>
Updates, Snow Creator, single DB load on startup. Smaller fixes
</commit_message>
<xml_diff>
--- a/database_copy.xlsx
+++ b/database_copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="1000" firstSheet="9" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Lod0_Region" sheetId="21" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2627" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="987">
   <si>
     <t>ID</t>
   </si>
@@ -2863,12 +2863,6 @@
     <t>TempMeltFactor</t>
   </si>
   <si>
-    <t>AlbedoMin</t>
-  </si>
-  <si>
-    <t>AlbedoMax</t>
-  </si>
-  <si>
     <t>tau_a</t>
   </si>
   <si>
@@ -2914,9 +2908,6 @@
     <t>OHMThresh_WD</t>
   </si>
   <si>
-    <t>ESTMCode</t>
-  </si>
-  <si>
     <t>Snow3</t>
   </si>
   <si>
@@ -2984,6 +2975,36 @@
   </si>
   <si>
     <t>Coastal large City</t>
+  </si>
+  <si>
+    <t>Alb16</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>SnowA</t>
+  </si>
+  <si>
+    <t>ANOHM15</t>
+  </si>
+  <si>
+    <t>Snow Hill, Antarctic</t>
+  </si>
+  <si>
+    <t>OHM15</t>
+  </si>
+  <si>
+    <t>Em11245</t>
+  </si>
+  <si>
+    <t>Alb17</t>
+  </si>
+  <si>
+    <t>SnowB</t>
+  </si>
+  <si>
+    <t>Yokohama, Japan</t>
   </si>
 </sst>
 </file>
@@ -3441,26 +3462,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.54296875" customWidth="1"/>
-    <col min="5" max="8" width="15.81640625" customWidth="1"/>
-    <col min="9" max="9" width="19.90625" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" customWidth="1"/>
-    <col min="11" max="11" width="21.36328125" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" customWidth="1"/>
-    <col min="13" max="13" width="23.1796875" customWidth="1"/>
-    <col min="14" max="14" width="18.54296875" customWidth="1"/>
-    <col min="15" max="15" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" customWidth="1"/>
+    <col min="5" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="15.81640625" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3513,18 +3534,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="B2" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C2" t="s">
         <v>629</v>
       </c>
       <c r="D2" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="E2" t="s">
         <v>782</v>
@@ -3563,21 +3584,21 @@
         <v>776</v>
       </c>
       <c r="Q2" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>968</v>
+      </c>
+      <c r="B3" t="s">
+        <v>969</v>
+      </c>
+      <c r="C3" t="s">
+        <v>970</v>
+      </c>
+      <c r="D3" t="s">
         <v>971</v>
-      </c>
-      <c r="B3" t="s">
-        <v>972</v>
-      </c>
-      <c r="C3" t="s">
-        <v>973</v>
-      </c>
-      <c r="D3" t="s">
-        <v>974</v>
       </c>
       <c r="E3" t="s">
         <v>783</v>
@@ -3616,15 +3637,15 @@
         <v>776</v>
       </c>
       <c r="Q3" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>974</v>
+      </c>
+      <c r="B4" t="s">
         <v>975</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>977</v>
-      </c>
-      <c r="B4" t="s">
-        <v>978</v>
       </c>
       <c r="C4" t="s">
         <v>631</v>
@@ -3669,7 +3690,7 @@
         <v>776</v>
       </c>
       <c r="Q4" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
   </sheetData>
@@ -3679,15 +3700,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q39" sqref="Q39"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3719,7 +3740,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>386</v>
       </c>
@@ -3751,7 +3772,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>388</v>
       </c>
@@ -3783,7 +3804,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>389</v>
       </c>
@@ -3815,7 +3836,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>391</v>
       </c>
@@ -3847,7 +3868,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>523</v>
       </c>
@@ -3879,7 +3900,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>524</v>
       </c>
@@ -3911,7 +3932,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>525</v>
       </c>
@@ -3943,7 +3964,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>526</v>
       </c>
@@ -3975,7 +3996,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>527</v>
       </c>
@@ -4007,7 +4028,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>528</v>
       </c>
@@ -4039,7 +4060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>529</v>
       </c>
@@ -4071,7 +4092,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>530</v>
       </c>
@@ -4103,7 +4124,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>531</v>
       </c>
@@ -4135,7 +4156,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>532</v>
       </c>
@@ -4165,6 +4186,38 @@
       </c>
       <c r="J15" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>982</v>
+      </c>
+      <c r="B16" t="s">
+        <v>978</v>
+      </c>
+      <c r="C16" t="s">
+        <v>978</v>
+      </c>
+      <c r="D16" t="s">
+        <v>978</v>
+      </c>
+      <c r="E16" t="s">
+        <v>771</v>
+      </c>
+      <c r="F16" t="s">
+        <v>387</v>
+      </c>
+      <c r="G16">
+        <v>0.25</v>
+      </c>
+      <c r="H16">
+        <v>0.6</v>
+      </c>
+      <c r="I16">
+        <v>-30</v>
+      </c>
+      <c r="J16" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4174,19 +4227,19 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R39" sqref="R39"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4212,7 +4265,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>394</v>
       </c>
@@ -4238,7 +4291,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>396</v>
       </c>
@@ -4264,7 +4317,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>397</v>
       </c>
@@ -4290,7 +4343,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>398</v>
       </c>
@@ -4316,7 +4369,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>399</v>
       </c>
@@ -4342,7 +4395,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>400</v>
       </c>
@@ -4368,7 +4421,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>401</v>
       </c>
@@ -4394,7 +4447,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>402</v>
       </c>
@@ -4420,7 +4473,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>403</v>
       </c>
@@ -4446,7 +4499,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>404</v>
       </c>
@@ -4472,7 +4525,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>405</v>
       </c>
@@ -4498,7 +4551,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>406</v>
       </c>
@@ -4524,7 +4577,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>498</v>
       </c>
@@ -4550,7 +4603,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>516</v>
       </c>
@@ -4576,7 +4629,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>658</v>
       </c>
@@ -4600,6 +4653,58 @@
       </c>
       <c r="H16" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="B17" t="s">
+        <v>978</v>
+      </c>
+      <c r="C17" t="s">
+        <v>978</v>
+      </c>
+      <c r="D17" t="s">
+        <v>979</v>
+      </c>
+      <c r="E17" t="s">
+        <v>487</v>
+      </c>
+      <c r="F17">
+        <v>0.18</v>
+      </c>
+      <c r="G17">
+        <v>0.85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="B18" t="s">
+        <v>978</v>
+      </c>
+      <c r="C18" t="s">
+        <v>978</v>
+      </c>
+      <c r="D18" t="s">
+        <v>985</v>
+      </c>
+      <c r="E18" t="s">
+        <v>986</v>
+      </c>
+      <c r="F18">
+        <v>0.18</v>
+      </c>
+      <c r="G18">
+        <v>0.8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4609,15 +4714,15 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4649,7 +4754,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>575</v>
       </c>
@@ -4681,7 +4786,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>576</v>
       </c>
@@ -4713,7 +4818,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>577</v>
       </c>
@@ -4745,7 +4850,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>578</v>
       </c>
@@ -4777,7 +4882,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>579</v>
       </c>
@@ -4809,7 +4914,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>580</v>
       </c>
@@ -4841,7 +4946,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>581</v>
       </c>
@@ -4873,7 +4978,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>582</v>
       </c>
@@ -4905,7 +5010,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>583</v>
       </c>
@@ -4937,7 +5042,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>584</v>
       </c>
@@ -4969,7 +5074,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>585</v>
       </c>
@@ -5001,7 +5106,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>586</v>
       </c>
@@ -5033,7 +5138,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>587</v>
       </c>
@@ -5065,7 +5170,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>588</v>
       </c>
@@ -5095,6 +5200,38 @@
       </c>
       <c r="J15" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B16" t="s">
+        <v>978</v>
+      </c>
+      <c r="C16" t="s">
+        <v>978</v>
+      </c>
+      <c r="D16" t="s">
+        <v>979</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="s">
+        <v>387</v>
+      </c>
+      <c r="G16">
+        <v>100000</v>
+      </c>
+      <c r="H16">
+        <v>1.2</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5111,9 +5248,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5157,7 +5294,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>592</v>
       </c>
@@ -5201,7 +5338,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>593</v>
       </c>
@@ -5245,7 +5382,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>594</v>
       </c>
@@ -5289,7 +5426,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>595</v>
       </c>
@@ -5333,7 +5470,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>596</v>
       </c>
@@ -5377,7 +5514,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>597</v>
       </c>
@@ -5421,10 +5558,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
   </sheetData>
@@ -5440,9 +5577,9 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5471,7 +5608,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>410</v>
       </c>
@@ -5500,7 +5637,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>411</v>
       </c>
@@ -5529,7 +5666,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>412</v>
       </c>
@@ -5558,7 +5695,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>446</v>
       </c>
@@ -5587,7 +5724,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>535</v>
       </c>
@@ -5616,7 +5753,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>536</v>
       </c>
@@ -5645,7 +5782,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>537</v>
       </c>
@@ -5674,7 +5811,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>538</v>
       </c>
@@ -5703,7 +5840,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>539</v>
       </c>
@@ -5732,7 +5869,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>540</v>
       </c>
@@ -5761,7 +5898,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>541</v>
       </c>
@@ -5790,7 +5927,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>542</v>
       </c>
@@ -5819,7 +5956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>543</v>
       </c>
@@ -5848,7 +5985,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>544</v>
       </c>
@@ -5886,18 +6023,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="17.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5923,7 +6058,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>415</v>
       </c>
@@ -5949,7 +6084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>416</v>
       </c>
@@ -5975,7 +6110,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>417</v>
       </c>
@@ -6001,7 +6136,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>445</v>
       </c>
@@ -6027,7 +6162,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>545</v>
       </c>
@@ -6053,7 +6188,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>546</v>
       </c>
@@ -6079,7 +6214,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>547</v>
       </c>
@@ -6105,7 +6240,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>548</v>
       </c>
@@ -6131,7 +6266,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>549</v>
       </c>
@@ -6157,7 +6292,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>550</v>
       </c>
@@ -6183,7 +6318,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>551</v>
       </c>
@@ -6209,7 +6344,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>552</v>
       </c>
@@ -6235,7 +6370,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>553</v>
       </c>
@@ -6261,7 +6396,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>554</v>
       </c>
@@ -6300,9 +6435,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6358,7 +6493,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>424</v>
       </c>
@@ -6414,7 +6549,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>425</v>
       </c>
@@ -6470,7 +6605,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>426</v>
       </c>
@@ -6526,7 +6661,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>427</v>
       </c>
@@ -6537,7 +6672,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="E5" t="s">
         <v>476</v>
@@ -6595,18 +6730,18 @@
       <selection activeCell="E2" sqref="D2:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.54296875" customWidth="1"/>
-    <col min="4" max="4" width="29.54296875" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6638,7 +6773,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>435</v>
       </c>
@@ -6670,7 +6805,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>438</v>
       </c>
@@ -6702,7 +6837,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>442</v>
       </c>
@@ -6734,7 +6869,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>447</v>
       </c>
@@ -6766,7 +6901,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>555</v>
       </c>
@@ -6798,7 +6933,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>556</v>
       </c>
@@ -6843,12 +6978,12 @@
       <selection activeCell="E2" sqref="E2:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="28.81640625" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6880,7 +7015,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>436</v>
       </c>
@@ -6912,7 +7047,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>439</v>
       </c>
@@ -6944,7 +7079,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>443</v>
       </c>
@@ -6976,7 +7111,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>448</v>
       </c>
@@ -7008,7 +7143,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>557</v>
       </c>
@@ -7040,7 +7175,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>558</v>
       </c>
@@ -7072,7 +7207,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>559</v>
       </c>
@@ -7104,7 +7239,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>560</v>
       </c>
@@ -7136,7 +7271,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>561</v>
       </c>
@@ -7168,7 +7303,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>562</v>
       </c>
@@ -7200,7 +7335,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>563</v>
       </c>
@@ -7232,7 +7367,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>564</v>
       </c>
@@ -7264,7 +7399,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>565</v>
       </c>
@@ -7296,7 +7431,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>566</v>
       </c>
@@ -7341,13 +7476,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="17.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.54296875" customWidth="1"/>
+    <col min="1" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7370,7 +7505,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>612</v>
       </c>
@@ -7393,7 +7528,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>620</v>
       </c>
@@ -7416,7 +7551,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>622</v>
       </c>
@@ -7439,7 +7574,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>623</v>
       </c>
@@ -7475,15 +7610,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
-    <col min="3" max="3" width="34.54296875" customWidth="1"/>
-    <col min="7" max="7" width="66.453125" customWidth="1"/>
-    <col min="14" max="14" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="66.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7527,7 +7662,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7571,7 +7706,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7615,7 +7750,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -7659,7 +7794,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -7703,7 +7838,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -7744,7 +7879,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -7782,7 +7917,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -7823,7 +7958,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -7861,7 +7996,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -7899,7 +8034,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -7940,7 +8075,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -7978,7 +8113,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -8019,7 +8154,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -8057,7 +8192,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -8095,7 +8230,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -8133,7 +8268,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -8177,7 +8312,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -8221,7 +8356,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -8276,12 +8411,12 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8307,8 +8442,8 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>641</v>
       </c>
       <c r="B2" t="s">
@@ -8333,8 +8468,8 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>660</v>
       </c>
       <c r="B3" t="s">
@@ -8359,8 +8494,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>661</v>
       </c>
       <c r="B4" t="s">
@@ -8385,8 +8520,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>664</v>
       </c>
       <c r="B5" t="s">
@@ -8420,16 +8555,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:57" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8602,7 +8737,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>669</v>
       </c>
@@ -8775,7 +8910,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>670</v>
       </c>
@@ -8945,7 +9080,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>671</v>
       </c>
@@ -9118,7 +9253,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>672</v>
       </c>
@@ -9288,7 +9423,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>673</v>
       </c>
@@ -9458,7 +9593,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>674</v>
       </c>
@@ -9628,7 +9763,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>675</v>
       </c>
@@ -9798,7 +9933,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>676</v>
       </c>
@@ -9968,7 +10103,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>677</v>
       </c>
@@ -10138,7 +10273,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>678</v>
       </c>
@@ -10308,7 +10443,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>679</v>
       </c>
@@ -10478,7 +10613,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>680</v>
       </c>
@@ -10648,7 +10783,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>681</v>
       </c>
@@ -10818,7 +10953,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>735</v>
       </c>
@@ -10988,7 +11123,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>736</v>
       </c>
@@ -11158,7 +11293,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>737</v>
       </c>
@@ -11328,7 +11463,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>738</v>
       </c>
@@ -11498,21 +11633,21 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>739</v>
       </c>
       <c r="B19" t="s">
-        <v>482</v>
+        <v>978</v>
       </c>
       <c r="C19" t="s">
-        <v>482</v>
+        <v>978</v>
       </c>
       <c r="D19" t="s">
-        <v>759</v>
+        <v>978</v>
       </c>
       <c r="E19" t="s">
-        <v>762</v>
+        <v>981</v>
       </c>
       <c r="F19">
         <v>1.1000000000000001</v>
@@ -11668,7 +11803,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>740</v>
       </c>
@@ -11838,7 +11973,7 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>741</v>
       </c>
@@ -12019,17 +12154,17 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12124,15 +12259,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>775</v>
       </c>
       <c r="B2" t="s">
         <v>766</v>
       </c>
       <c r="C2" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="D2" t="s">
         <v>764</v>
@@ -12219,15 +12354,15 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>776</v>
       </c>
       <c r="B3" t="s">
         <v>766</v>
       </c>
       <c r="C3" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="D3" t="s">
         <v>765</v>
@@ -12314,8 +12449,8 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>777</v>
       </c>
       <c r="B4" t="s">
@@ -12406,8 +12541,8 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>778</v>
       </c>
       <c r="B5" t="s">
@@ -12498,8 +12633,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>779</v>
       </c>
       <c r="B6" t="s">
@@ -12590,8 +12725,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>780</v>
       </c>
       <c r="B7" t="s">
@@ -12682,8 +12817,8 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>781</v>
       </c>
       <c r="B8" t="s">
@@ -12774,15 +12909,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>782</v>
       </c>
       <c r="B9" t="s">
         <v>766</v>
       </c>
       <c r="C9" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="D9" t="s">
         <v>764</v>
@@ -12866,15 +13001,15 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>783</v>
       </c>
       <c r="B10" t="s">
         <v>766</v>
       </c>
       <c r="C10" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="D10" t="s">
         <v>765</v>
@@ -12958,8 +13093,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>784</v>
       </c>
       <c r="B11" t="s">
@@ -13050,8 +13185,8 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>785</v>
       </c>
       <c r="B12" t="s">
@@ -13142,8 +13277,8 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>786</v>
       </c>
       <c r="B13" t="s">
@@ -13234,8 +13369,8 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>787</v>
       </c>
       <c r="B14" t="s">
@@ -13326,8 +13461,8 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>788</v>
       </c>
       <c r="B15" t="s">
@@ -13418,8 +13553,8 @@
         <v>-999</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>789</v>
       </c>
       <c r="B16" t="s">
@@ -13510,8 +13645,8 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>790</v>
       </c>
       <c r="B17" t="s">
@@ -13602,8 +13737,8 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>791</v>
       </c>
       <c r="B18" t="s">
@@ -13694,8 +13829,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>792</v>
       </c>
       <c r="B19" t="s">
@@ -13786,8 +13921,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>793</v>
       </c>
       <c r="B20" t="s">
@@ -13878,8 +14013,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>794</v>
       </c>
       <c r="B21" t="s">
@@ -13980,12 +14115,12 @@
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14074,8 +14209,8 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>822</v>
       </c>
       <c r="B2" t="s">
@@ -14163,8 +14298,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>823</v>
       </c>
       <c r="B3" t="s">
@@ -14252,8 +14387,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>824</v>
       </c>
       <c r="B4" t="s">
@@ -14341,8 +14476,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>825</v>
       </c>
       <c r="B5" t="s">
@@ -14437,15 +14572,15 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14462,81 +14597,72 @@
         <v>938</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>939</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>941</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>942</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>944</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>945</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>946</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>948</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>950</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>951</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>953</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>954</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>955</v>
+        <v>854</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B2" t="s">
         <v>956</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>935</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>959</v>
-      </c>
-      <c r="C2" t="s">
-        <v>962</v>
       </c>
       <c r="D2">
         <v>1.6000000000000001E-3</v>
@@ -14544,82 +14670,73 @@
       <c r="E2">
         <v>0.12</v>
       </c>
-      <c r="F2">
-        <v>0.18</v>
-      </c>
-      <c r="G2">
-        <v>0.85</v>
+      <c r="F2" t="s">
+        <v>977</v>
+      </c>
+      <c r="G2" t="s">
+        <v>983</v>
       </c>
       <c r="H2">
-        <v>0.99</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="I2">
-        <v>1.7999999999999999E-2</v>
+        <v>0.11</v>
       </c>
       <c r="J2">
-        <v>0.11</v>
+        <v>2</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="M2">
-        <v>400</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="N2">
-        <v>4.2999999999999997E-2</v>
+        <v>0.05</v>
       </c>
       <c r="O2">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="P2">
-        <v>0.2</v>
-      </c>
-      <c r="Q2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R2">
-        <v>61</v>
-      </c>
-      <c r="S2">
-        <v>61</v>
-      </c>
-      <c r="T2">
-        <v>61</v>
+      <c r="Q2" t="s">
+        <v>982</v>
+      </c>
+      <c r="R2" t="s">
+        <v>982</v>
+      </c>
+      <c r="S2" t="s">
+        <v>982</v>
+      </c>
+      <c r="T2" t="s">
+        <v>982</v>
       </c>
       <c r="U2">
-        <v>61</v>
+        <v>-999</v>
       </c>
       <c r="V2">
-        <v>10</v>
-      </c>
-      <c r="W2">
-        <v>0.9</v>
-      </c>
-      <c r="X2">
-        <v>61</v>
-      </c>
-      <c r="Y2">
-        <v>100000</v>
-      </c>
-      <c r="Z2">
-        <v>1.2</v>
-      </c>
-      <c r="AA2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+        <v>-999</v>
+      </c>
+      <c r="W2" t="s">
+        <v>739</v>
+      </c>
+      <c r="X2" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>936</v>
       </c>
       <c r="B3" t="s">
         <v>476</v>
       </c>
       <c r="C3" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="D3">
         <v>1E-3</v>
@@ -14627,79 +14744,70 @@
       <c r="E3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F3">
-        <v>0.18</v>
-      </c>
-      <c r="G3">
-        <v>0.8</v>
+      <c r="F3" t="s">
+        <v>984</v>
+      </c>
+      <c r="G3" t="s">
+        <v>983</v>
       </c>
       <c r="H3">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
       <c r="I3">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>450</v>
+      </c>
+      <c r="M3">
+        <v>0.02</v>
+      </c>
+      <c r="N3">
+        <v>0.03</v>
+      </c>
+      <c r="O3">
         <v>0.1</v>
       </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="M3">
-        <v>450</v>
-      </c>
-      <c r="N3">
-        <v>0.02</v>
-      </c>
-      <c r="O3">
-        <v>0.03</v>
-      </c>
       <c r="P3">
-        <v>0.1</v>
-      </c>
-      <c r="Q3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R3">
-        <v>61</v>
-      </c>
-      <c r="S3">
-        <v>61</v>
-      </c>
-      <c r="T3">
-        <v>61</v>
+      <c r="Q3" t="s">
+        <v>982</v>
+      </c>
+      <c r="R3" t="s">
+        <v>982</v>
+      </c>
+      <c r="S3" t="s">
+        <v>982</v>
+      </c>
+      <c r="T3" t="s">
+        <v>982</v>
       </c>
       <c r="U3">
-        <v>61</v>
+        <v>-999</v>
       </c>
       <c r="V3">
-        <v>10</v>
-      </c>
-      <c r="W3">
-        <v>0.9</v>
-      </c>
-      <c r="X3">
-        <v>61</v>
-      </c>
-      <c r="Y3">
-        <v>100000</v>
-      </c>
-      <c r="Z3">
-        <v>1.2</v>
-      </c>
-      <c r="AA3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+        <v>-999</v>
+      </c>
+      <c r="W3" t="s">
+        <v>739</v>
+      </c>
+      <c r="X3" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B4" t="s">
         <v>957</v>
-      </c>
-      <c r="B4" t="s">
-        <v>960</v>
       </c>
       <c r="C4" t="s">
         <v>387</v>
@@ -14710,82 +14818,73 @@
       <c r="E4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F4">
-        <v>0.18</v>
-      </c>
-      <c r="G4">
-        <v>0.8</v>
+      <c r="F4" t="s">
+        <v>977</v>
+      </c>
+      <c r="G4" t="s">
+        <v>983</v>
       </c>
       <c r="H4">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
       <c r="I4">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>450</v>
+      </c>
+      <c r="M4">
+        <v>0.02</v>
+      </c>
+      <c r="N4">
+        <v>0.03</v>
+      </c>
+      <c r="O4">
         <v>0.1</v>
       </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4">
-        <v>450</v>
-      </c>
-      <c r="N4">
-        <v>0.02</v>
-      </c>
-      <c r="O4">
-        <v>0.03</v>
-      </c>
       <c r="P4">
-        <v>0.1</v>
-      </c>
-      <c r="Q4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R4">
-        <v>61</v>
-      </c>
-      <c r="S4">
-        <v>61</v>
-      </c>
-      <c r="T4">
-        <v>61</v>
+      <c r="Q4" t="s">
+        <v>982</v>
+      </c>
+      <c r="R4" t="s">
+        <v>982</v>
+      </c>
+      <c r="S4" t="s">
+        <v>982</v>
+      </c>
+      <c r="T4" t="s">
+        <v>982</v>
       </c>
       <c r="U4">
-        <v>61</v>
+        <v>-999</v>
       </c>
       <c r="V4">
-        <v>10</v>
-      </c>
-      <c r="W4">
-        <v>0.9</v>
-      </c>
-      <c r="X4">
-        <v>61</v>
-      </c>
-      <c r="Y4">
-        <v>100000</v>
-      </c>
-      <c r="Z4">
-        <v>1.2</v>
-      </c>
-      <c r="AA4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+        <v>-999</v>
+      </c>
+      <c r="W4" t="s">
+        <v>739</v>
+      </c>
+      <c r="X4" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="B5" t="s">
         <v>958</v>
       </c>
-      <c r="B5" t="s">
-        <v>961</v>
-      </c>
       <c r="C5" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -14793,71 +14892,62 @@
       <c r="E5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F5">
-        <v>0.18</v>
-      </c>
-      <c r="G5">
-        <v>0.8</v>
+      <c r="F5" t="s">
+        <v>984</v>
+      </c>
+      <c r="G5" t="s">
+        <v>983</v>
       </c>
       <c r="H5">
-        <v>0.99</v>
+        <v>0.01</v>
       </c>
       <c r="I5">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>450</v>
+      </c>
+      <c r="M5">
+        <v>0.02</v>
+      </c>
+      <c r="N5">
+        <v>0.03</v>
+      </c>
+      <c r="O5">
         <v>0.1</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-      <c r="M5">
-        <v>450</v>
-      </c>
-      <c r="N5">
-        <v>0.02</v>
-      </c>
-      <c r="O5">
-        <v>0.03</v>
-      </c>
       <c r="P5">
-        <v>0.1</v>
-      </c>
-      <c r="Q5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="R5">
-        <v>61</v>
-      </c>
-      <c r="S5">
-        <v>61</v>
-      </c>
-      <c r="T5">
-        <v>61</v>
+      <c r="Q5" t="s">
+        <v>982</v>
+      </c>
+      <c r="R5" t="s">
+        <v>982</v>
+      </c>
+      <c r="S5" t="s">
+        <v>982</v>
+      </c>
+      <c r="T5" t="s">
+        <v>982</v>
       </c>
       <c r="U5">
-        <v>61</v>
+        <v>-999</v>
       </c>
       <c r="V5">
-        <v>10</v>
-      </c>
-      <c r="W5">
-        <v>0.9</v>
-      </c>
-      <c r="X5">
-        <v>61</v>
-      </c>
-      <c r="Y5">
-        <v>100000</v>
-      </c>
-      <c r="Z5">
-        <v>1.2</v>
-      </c>
-      <c r="AA5">
-        <v>4</v>
+        <v>-999</v>
+      </c>
+      <c r="W5" t="s">
+        <v>739</v>
+      </c>
+      <c r="X5" t="s">
+        <v>980</v>
       </c>
     </row>
   </sheetData>
@@ -14870,15 +14960,15 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -14916,8 +15006,8 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>838</v>
       </c>
       <c r="B2" t="s">
@@ -14954,8 +15044,8 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>839</v>
       </c>
       <c r="B3" t="s">
@@ -14992,8 +15082,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>840</v>
       </c>
       <c r="B4" t="s">
@@ -15030,8 +15120,8 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>841</v>
       </c>
       <c r="B5" t="s">
@@ -15068,8 +15158,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>842</v>
       </c>
       <c r="B6" t="s">
@@ -15106,8 +15196,8 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>843</v>
       </c>
       <c r="B7" t="s">
@@ -15144,8 +15234,8 @@
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>844</v>
       </c>
       <c r="B8" t="s">
@@ -15182,8 +15272,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>845</v>
       </c>
       <c r="B9" t="s">
@@ -15230,16 +15320,16 @@
   <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15364,8 +15454,8 @@
         <v>900</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>901</v>
       </c>
       <c r="B2" t="s">
@@ -15489,8 +15579,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>903</v>
       </c>
       <c r="B3" t="s">
@@ -15614,8 +15704,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>902</v>
       </c>
       <c r="B4" t="s">
@@ -15739,8 +15829,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>904</v>
       </c>
       <c r="B5" t="s">
@@ -15864,8 +15954,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>905</v>
       </c>
       <c r="B6" t="s">
@@ -15989,8 +16079,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>906</v>
       </c>
       <c r="B7" t="s">
@@ -16114,8 +16204,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>907</v>
       </c>
       <c r="B8" t="s">
@@ -16239,8 +16329,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>908</v>
       </c>
       <c r="B9" t="s">
@@ -16364,8 +16454,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>909</v>
       </c>
       <c r="B10" t="s">
@@ -16489,8 +16579,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>910</v>
       </c>
       <c r="B11" t="s">
@@ -16627,17 +16717,17 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.1796875" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="12" max="12" width="20.453125" customWidth="1"/>
-    <col min="13" max="13" width="15.1796875" customWidth="1"/>
-    <col min="14" max="14" width="17.54296875" customWidth="1"/>
-    <col min="15" max="15" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16699,7 +16789,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -16752,7 +16842,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -16805,7 +16895,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -16858,7 +16948,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -16911,7 +17001,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -16964,7 +17054,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -17017,7 +17107,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -17070,7 +17160,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -17123,7 +17213,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -17176,7 +17266,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -17229,7 +17319,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -17282,7 +17372,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -17348,9 +17438,9 @@
       <selection activeCell="M9" sqref="L9:M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17397,7 +17487,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>491</v>
       </c>
@@ -17444,7 +17534,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>567</v>
       </c>
@@ -17504,14 +17594,14 @@
       <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17562,7 +17652,7 @@
       </c>
       <c r="Q1" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -17606,7 +17696,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -17650,7 +17740,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -17694,7 +17784,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -17738,7 +17828,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>465</v>
       </c>
@@ -17782,7 +17872,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>466</v>
       </c>
@@ -17826,7 +17916,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>467</v>
       </c>
@@ -17870,7 +17960,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>469</v>
       </c>
@@ -17914,7 +18004,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>470</v>
       </c>
@@ -17958,7 +18048,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>488</v>
       </c>
@@ -18002,7 +18092,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>489</v>
       </c>
@@ -18059,9 +18149,9 @@
       <selection activeCell="A37" sqref="A37:A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -18102,7 +18192,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -18128,7 +18218,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>73</v>
       </c>
@@ -18157,7 +18247,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>80</v>
       </c>
@@ -18189,7 +18279,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>86</v>
       </c>
@@ -18221,7 +18311,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
@@ -18250,7 +18340,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>97</v>
       </c>
@@ -18279,7 +18369,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
@@ -18311,7 +18401,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>107</v>
       </c>
@@ -18343,7 +18433,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
@@ -18372,7 +18462,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>118</v>
       </c>
@@ -18404,7 +18494,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>123</v>
       </c>
@@ -18433,7 +18523,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>128</v>
       </c>
@@ -18465,7 +18555,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>134</v>
       </c>
@@ -18497,7 +18587,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>139</v>
       </c>
@@ -18529,7 +18619,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>144</v>
       </c>
@@ -18561,7 +18651,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>149</v>
       </c>
@@ -18593,7 +18683,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>154</v>
       </c>
@@ -18622,7 +18712,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>158</v>
       </c>
@@ -18642,7 +18732,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>162</v>
       </c>
@@ -18674,7 +18764,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>168</v>
       </c>
@@ -18706,7 +18796,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>173</v>
       </c>
@@ -18738,7 +18828,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>178</v>
       </c>
@@ -18761,7 +18851,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>183</v>
       </c>
@@ -18793,7 +18883,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>189</v>
       </c>
@@ -18816,7 +18906,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>194</v>
       </c>
@@ -18848,7 +18938,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>199</v>
       </c>
@@ -18880,7 +18970,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>204</v>
       </c>
@@ -18912,7 +19002,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>209</v>
       </c>
@@ -18944,7 +19034,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>215</v>
       </c>
@@ -18970,7 +19060,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>221</v>
       </c>
@@ -19005,7 +19095,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>230</v>
       </c>
@@ -19037,7 +19127,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>236</v>
       </c>
@@ -19069,7 +19159,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>241</v>
       </c>
@@ -19101,7 +19191,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>247</v>
       </c>
@@ -19133,7 +19223,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>253</v>
       </c>
@@ -19165,7 +19255,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>259</v>
       </c>
@@ -19194,7 +19284,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>264</v>
       </c>
@@ -19226,7 +19316,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>269</v>
       </c>
@@ -19258,7 +19348,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>275</v>
       </c>
@@ -19290,7 +19380,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>280</v>
       </c>
@@ -19322,7 +19412,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>285</v>
       </c>
@@ -19354,7 +19444,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>292</v>
       </c>
@@ -19383,7 +19473,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>298</v>
       </c>
@@ -19403,7 +19493,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>302</v>
       </c>
@@ -19435,7 +19525,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>307</v>
       </c>
@@ -19464,7 +19554,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>312</v>
       </c>
@@ -19496,7 +19586,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>318</v>
       </c>
@@ -19528,7 +19618,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>324</v>
       </c>
@@ -19554,7 +19644,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>330</v>
       </c>
@@ -19586,7 +19676,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>335</v>
       </c>
@@ -19618,7 +19708,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>340</v>
       </c>
@@ -19650,7 +19740,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>346</v>
       </c>
@@ -19679,7 +19769,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>352</v>
       </c>
@@ -19711,7 +19801,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>616</v>
       </c>
@@ -19741,15 +19831,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19772,7 +19862,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>362</v>
       </c>
@@ -19795,7 +19885,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>366</v>
       </c>
@@ -19818,7 +19908,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>368</v>
       </c>
@@ -19841,7 +19931,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>370</v>
       </c>
@@ -19864,7 +19954,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>373</v>
       </c>
@@ -19887,7 +19977,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>375</v>
       </c>
@@ -19910,7 +20000,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>376</v>
       </c>
@@ -19933,7 +20023,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>377</v>
       </c>
@@ -19956,7 +20046,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>378</v>
       </c>
@@ -19979,7 +20069,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>379</v>
       </c>
@@ -20002,7 +20092,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>381</v>
       </c>
@@ -20025,7 +20115,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>493</v>
       </c>
@@ -20048,7 +20138,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>533</v>
       </c>
@@ -20071,7 +20161,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>534</v>
       </c>
@@ -20094,7 +20184,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>667</v>
       </c>
@@ -20114,6 +20204,29 @@
         <v>0.78830303030303095</v>
       </c>
       <c r="G16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B17" t="s">
+        <v>978</v>
+      </c>
+      <c r="C17" t="s">
+        <v>978</v>
+      </c>
+      <c r="D17" t="s">
+        <v>979</v>
+      </c>
+      <c r="E17" t="s">
+        <v>522</v>
+      </c>
+      <c r="F17">
+        <v>0.99</v>
+      </c>
+      <c r="G17" t="s">
         <v>73</v>
       </c>
     </row>
@@ -20130,9 +20243,9 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -20164,7 +20277,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>574</v>
       </c>
@@ -20196,7 +20309,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>624</v>
       </c>
@@ -20228,7 +20341,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>625</v>
       </c>
@@ -20260,7 +20373,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>626</v>
       </c>
@@ -20305,14 +20418,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.453125" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20332,7 +20445,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>852</v>
       </c>
@@ -20352,7 +20465,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>853</v>
       </c>

</xml_diff>